<commit_message>
updated spreadsheet with standard deviation data
</commit_message>
<xml_diff>
--- a/results/Performance Tracking.xlsx
+++ b/results/Performance Tracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+  <si>
+    <t xml:space="preserve">Early models before performance analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Late models with standard deviation analysis</t>
+  </si>
   <si>
     <t xml:space="preserve">Version</t>
   </si>
@@ -28,15 +34,21 @@
     <t xml:space="preserve">Time </t>
   </si>
   <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard deviation from center line (100 seconds per lane)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simulation</t>
   </si>
   <si>
     <t xml:space="preserve">Network</t>
   </si>
   <si>
-    <t xml:space="preserve">Model</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test 1</t>
   </si>
   <si>
@@ -55,6 +67,33 @@
     <t xml:space="preserve">Average</t>
   </si>
   <si>
+    <t xml:space="preserve">File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
     <t xml:space="preserve">48a63c1</t>
   </si>
   <si>
@@ -67,6 +106,15 @@
     <t xml:space="preserve">N/A</t>
   </si>
   <si>
+    <t xml:space="preserve">1503482632.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dense, small filters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falls off track in 9.4 seconds</t>
+  </si>
+  <si>
     <t xml:space="preserve">be3a4f9</t>
   </si>
   <si>
@@ -76,6 +124,12 @@
     <t xml:space="preserve">1500310252.h5</t>
   </si>
   <si>
+    <t xml:space="preserve">1503486349.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NVIDIA</t>
+  </si>
+  <si>
     <t xml:space="preserve">e9e789a</t>
   </si>
   <si>
@@ -85,6 +139,15 @@
     <t xml:space="preserve">1500327174.h5</t>
   </si>
   <si>
+    <t xml:space="preserve">1503488664.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIT DeepTesla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falls off track in 5.1 seconds</t>
+  </si>
+  <si>
     <t xml:space="preserve">4a377a4</t>
   </si>
   <si>
@@ -94,6 +157,15 @@
     <t xml:space="preserve">1500416566.h5</t>
   </si>
   <si>
+    <t xml:space="preserve">1503537792.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many filters, few layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Falls off track in 27.4 seconds</t>
+  </si>
+  <si>
     <t xml:space="preserve">0915d0e</t>
   </si>
   <si>
@@ -104,15 +176,22 @@
   </si>
   <si>
     <t xml:space="preserve">Model successfully drives around entire track.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1503559070.h5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many filters, many layers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -185,7 +264,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -195,6 +274,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -215,196 +298,340 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6122448979592"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="19" min="15" style="1" width="13.4744897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>8.28</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>8.12</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>8.3</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>8.12</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <f aca="false">AVERAGE(D3:G3)</f>
-        <v>8.205</v>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>38.56</v>
+        <v>8.28</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>32.42</v>
+        <v>8.12</v>
       </c>
       <c r="F4" s="1" t="n">
-        <v>22.86</v>
+        <v>8.3</v>
       </c>
       <c r="G4" s="1" t="n">
-        <v>30.28</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>76.08</v>
+        <v>8.12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="I4" s="1" t="n">
-        <f aca="false">AVERAGE(D4:H4)</f>
-        <v>40.04</v>
+        <f aca="false">AVERAGE(D4:G4)</f>
+        <v>8.205</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4" s="3" t="n">
+        <v>0.00011863</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>0.00011548</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>9.74</v>
+        <v>38.56</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>7.94</v>
+        <v>32.42</v>
       </c>
       <c r="F5" s="1" t="n">
-        <v>8.62</v>
+        <v>22.86</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>7.58</v>
+        <v>30.28</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>7.82</v>
+        <v>76.08</v>
       </c>
       <c r="I5" s="1" t="n">
         <f aca="false">AVERAGE(D5:H5)</f>
-        <v>8.34</v>
+        <v>40.04</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="3" t="n">
+        <v>3.9121E-006</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>7.3941E-006</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>0.7443967</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>0.224663</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>0.6361409</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>0.810182</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <f aca="false">AVERAGE(O5:R5)</f>
+        <v>0.60384565</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>15.88</v>
+        <v>9.74</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>15.6</v>
+        <v>7.94</v>
       </c>
       <c r="F6" s="1" t="n">
-        <v>16.34</v>
+        <v>8.62</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>14.84</v>
+        <v>7.58</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>14.78</v>
+        <v>7.82</v>
       </c>
       <c r="I6" s="1" t="n">
         <f aca="false">AVERAGE(D6:H6)</f>
-        <v>15.488</v>
+        <v>8.34</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="3" t="n">
+        <v>5.8032E-005</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>5.9841E-005</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>15.88</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>16.34</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>14.84</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>14.78</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <f aca="false">AVERAGE(D7:H7)</f>
+        <v>15.488</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M7" s="3" t="n">
+        <v>0.00011773</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>0.00012194</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M8" s="3" t="n">
+        <v>3.1948E-007</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>7.9591E-006</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>0.7085852</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>0.3898657</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>0.6391341</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>0.8785638</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <f aca="false">AVERAGE(O8:R8)</f>
+        <v>0.6540372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added low pass filter data to spreadsheet
</commit_message>
<xml_diff>
--- a/results/Performance Tracking.xlsx
+++ b/results/Performance Tracking.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t xml:space="preserve">Early models before performance analysis</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Late models with standard deviation analysis</t>
   </si>
   <si>
+    <t xml:space="preserve">Standard deviations for low pass filter parameters (using network 1503559070.h5)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Version</t>
   </si>
   <si>
@@ -43,6 +46,24 @@
     <t xml:space="preserve">Standard deviation from center line (100 seconds per lane)</t>
   </si>
   <si>
+    <t xml:space="preserve">Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lane 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simulation</t>
   </si>
   <si>
@@ -79,19 +100,7 @@
     <t xml:space="preserve">Validation</t>
   </si>
   <si>
-    <t xml:space="preserve">Lane 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lane 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean</t>
+    <t xml:space="preserve">Filter disabled</t>
   </si>
   <si>
     <t xml:space="preserve">48a63c1</t>
@@ -115,6 +124,9 @@
     <t xml:space="preserve">Falls off track in 9.4 seconds</t>
   </si>
   <si>
+    <t xml:space="preserve">1.0, 0.3, 0.2, 0.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">be3a4f9</t>
   </si>
   <si>
@@ -130,6 +142,9 @@
     <t xml:space="preserve">NVIDIA</t>
   </si>
   <si>
+    <t xml:space="preserve">1.0, 0.7, 0.6, 0.5, 0.4</t>
+  </si>
+  <si>
     <t xml:space="preserve">e9e789a</t>
   </si>
   <si>
@@ -146,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">Falls off track in 5.1 seconds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0, 0.8, 0.3, 0.1</t>
   </si>
   <si>
     <t xml:space="preserve">4a377a4</t>
@@ -298,116 +316,187 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O5" activeCellId="0" sqref="O5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="19" min="15" style="1" width="13.4744897959184"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="22.6428571428571"/>
+    <col collapsed="false" hidden="false" max="26" min="22" style="1" width="14.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="1" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
       <c r="K1" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
+      <c r="Q1" s="0"/>
+      <c r="R1" s="0"/>
+      <c r="S1" s="0"/>
+      <c r="U1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
       <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
       <c r="K2" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L2" s="0"/>
       <c r="M2" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="N2" s="0"/>
       <c r="O2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="U2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>23</v>
+      <c r="U3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>0.7085852</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>0.3898657</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>0.6391341</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>0.8785638</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <f aca="false">AVERAGE(V3:Y3)</f>
+        <v>0.6540372</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>8.28</v>
@@ -422,17 +511,17 @@
         <v>8.12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="n">
         <f aca="false">AVERAGE(D4:G4)</f>
         <v>8.205</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M4" s="3" t="n">
         <v>0.00011863</v>
@@ -441,18 +530,41 @@
         <v>0.00011548</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="P4" s="0"/>
+      <c r="Q4" s="0"/>
+      <c r="R4" s="0"/>
+      <c r="S4" s="0"/>
+      <c r="U4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" s="1" t="n">
+        <v>0.7065313</v>
+      </c>
+      <c r="W4" s="1" t="n">
+        <v>0.3907571</v>
+      </c>
+      <c r="X4" s="1" t="n">
+        <v>0.6443396</v>
+      </c>
+      <c r="Y4" s="1" t="n">
+        <v>0.9180865</v>
+      </c>
+      <c r="Z4" s="1" t="n">
+        <f aca="false">AVERAGE(V4:Y4)</f>
+        <v>0.664928625</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>38.56</v>
@@ -474,10 +586,10 @@
         <v>40.04</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="M5" s="3" t="n">
         <v>3.9121E-006</v>
@@ -501,16 +613,35 @@
         <f aca="false">AVERAGE(O5:R5)</f>
         <v>0.60384565</v>
       </c>
+      <c r="U5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>0.6531526</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>0.3540962</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>0.6581528</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>0.8799137</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <f aca="false">AVERAGE(V5:Y5)</f>
+        <v>0.636328825</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>9.74</v>
@@ -532,10 +663,10 @@
         <v>8.34</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="M6" s="3" t="n">
         <v>5.8032E-005</v>
@@ -544,18 +675,41 @@
         <v>5.9841E-005</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
+      </c>
+      <c r="P6" s="0"/>
+      <c r="Q6" s="0"/>
+      <c r="R6" s="0"/>
+      <c r="S6" s="0"/>
+      <c r="U6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>0.6268617</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>1.001549</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>0.650547</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>0.8531444</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <f aca="false">AVERAGE(V6:Y6)</f>
+        <v>0.783025525</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>15.88</v>
@@ -577,10 +731,10 @@
         <v>15.488</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="M7" s="3" t="n">
         <v>0.00011773</v>
@@ -589,27 +743,31 @@
         <v>0.00012194</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>47</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="P7" s="0"/>
+      <c r="Q7" s="0"/>
+      <c r="R7" s="0"/>
+      <c r="S7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="M8" s="3" t="n">
         <v>3.1948E-007</v>

</xml_diff>

<commit_message>
Updated spreadsheet, move auto drive screenshots to archive folder
</commit_message>
<xml_diff>
--- a/results/Performance Tracking.xlsx
+++ b/results/Performance Tracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="107">
   <si>
     <t xml:space="preserve">Early models before performance analysis</t>
   </si>
@@ -31,7 +31,10 @@
     <t xml:space="preserve">Standard deviations for low pass filter parameters (using network 1503559070.h5)</t>
   </si>
   <si>
-    <t xml:space="preserve">Learning curve (combined MacIsaac dataset), commit </t>
+    <t xml:space="preserve">Learning curve (combined MacIsaac dataset), commit 0fbd990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Real-world test runs</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
@@ -67,10 +70,34 @@
     <t xml:space="preserve">Mean</t>
   </si>
   <si>
+    <t xml:space="preserve">Trial#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network</t>
+  </si>
+  <si>
     <t xml:space="preserve">Optimizer</t>
   </si>
   <si>
-    <t xml:space="preserve">Images (approx)</t>
+    <t xml:space="preserve">Activation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dropout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch normalization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Batch size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#Layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Images</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epochs</t>
   </si>
   <si>
     <t xml:space="preserve">Train loss (ep. 5)</t>
@@ -79,12 +106,18 @@
     <t xml:space="preserve">Val loss (ep. 5)</t>
   </si>
   <si>
+    <t xml:space="preserve">TV Ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Background information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meters traveled before failure</t>
+  </si>
+  <si>
     <t xml:space="preserve">Simulation</t>
   </si>
   <si>
-    <t xml:space="preserve">Network</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test 1</t>
   </si>
   <si>
@@ -118,6 +151,51 @@
     <t xml:space="preserve">Filter disabled</t>
   </si>
   <si>
+    <t xml:space="preserve">Nvidia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adadelta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epoch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Val loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Std dev (visualizer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trial 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">48a63c1</t>
   </si>
   <si>
@@ -142,6 +220,18 @@
     <t xml:space="preserve">1.0, 0.3, 0.2, 0.1</t>
   </si>
   <si>
+    <t xml:space="preserve">Delki Dozzi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aug30-31-delki-second-dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21a73d3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Failed to steer whatsoever</t>
+  </si>
+  <si>
     <t xml:space="preserve">be3a4f9</t>
   </si>
   <si>
@@ -160,6 +250,15 @@
     <t xml:space="preserve">1.0, 0.7, 0.6, 0.5, 0.4</t>
   </si>
   <si>
+    <t xml:space="preserve">MacIsaac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sep2-3-macisaac-second-dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0fbd990</t>
+  </si>
+  <si>
     <t xml:space="preserve">e9e789a</t>
   </si>
   <si>
@@ -215,16 +314,46 @@
   </si>
   <si>
     <t xml:space="preserve">Many filters, many layers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removed last conv layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input, 0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SGD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second level analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Third level analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fourth level analysis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00E+00"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="169" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -250,8 +379,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Cantarell"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -297,7 +426,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -311,6 +440,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,32 +472,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AZ45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AF6" activeCellId="0" sqref="AF6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AJ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AW7" activeCellId="0" sqref="AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="25.515306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="14" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="26" min="22" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="16.9438775510204"/>
-    <col collapsed="false" hidden="false" max="30" min="29" style="1" width="17.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="31" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="10" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="24.9744897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="19" min="14" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="26" min="22" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="1" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="26.4591836734694"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="2" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="2" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="3" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="4" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="43" min="43" style="1" width="14.7244897959184"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="1" width="35.1530612244898"/>
+    <col collapsed="false" hidden="false" max="47" min="47" style="1" width="11.3928571428571"/>
+    <col collapsed="false" hidden="false" max="48" min="48" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="49" min="49" style="1" width="17.2244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="50" style="1" width="9.71938775510204"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -366,114 +523,155 @@
       <c r="U1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="AQ1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>18</v>
+      <c r="AF2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AW2" s="0"/>
+      <c r="AX2" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="V3" s="1" t="n">
         <v>0.7085852</v>
@@ -491,19 +689,89 @@
         <f aca="false">AVERAGE(V3:Y3)</f>
         <v>0.6540372</v>
       </c>
-      <c r="AC3" s="1" t="n">
+      <c r="AB3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK3" s="2" t="n">
         <v>5000</v>
+      </c>
+      <c r="AL3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM3" s="3" t="n">
+        <v>0.00045431</v>
+      </c>
+      <c r="AN3" s="3" t="n">
+        <v>0.0015</v>
+      </c>
+      <c r="AO3" s="4" t="n">
+        <f aca="false">AN3/AM3</f>
+        <v>3.30171028592811</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW3" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
+        <v>59</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>8.28</v>
@@ -518,17 +786,17 @@
         <v>8.12</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1" t="n">
         <f aca="false">AVERAGE(D4:G4)</f>
         <v>8.205</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="M4" s="3" t="n">
         <v>0.00011863</v>
@@ -537,10 +805,10 @@
         <v>0.00011548</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="V4" s="1" t="n">
         <v>0.7065313</v>
@@ -558,19 +826,81 @@
         <f aca="false">AVERAGE(V4:Y4)</f>
         <v>0.664928625</v>
       </c>
-      <c r="AC4" s="1" t="n">
+      <c r="AB4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK4" s="2" t="n">
         <v>10000</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM4" s="3" t="n">
+        <v>0.00043769</v>
+      </c>
+      <c r="AN4" s="3" t="n">
+        <v>0.00091329</v>
+      </c>
+      <c r="AO4" s="4" t="n">
+        <f aca="false">AN4/AM4</f>
+        <v>2.0866138134296</v>
+      </c>
+      <c r="AQ4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR4" s="6" t="n">
+        <v>42978</v>
+      </c>
+      <c r="AS4" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="AT4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU4" s="3" t="n">
+        <v>1.5862E-005</v>
+      </c>
+      <c r="AV4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AW4" s="0"/>
+      <c r="AX4" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>38.56</v>
@@ -592,10 +922,10 @@
         <v>40.04</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="M5" s="3" t="n">
         <v>3.9121E-006</v>
@@ -620,7 +950,7 @@
         <v>0.60384565</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="V5" s="1" t="n">
         <v>0.6531526</v>
@@ -638,19 +968,87 @@
         <f aca="false">AVERAGE(V5:Y5)</f>
         <v>0.636328825</v>
       </c>
-      <c r="AC5" s="1" t="n">
+      <c r="AB5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK5" s="2" t="n">
         <v>20000</v>
+      </c>
+      <c r="AL5" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM5" s="3" t="n">
+        <v>0.00035167</v>
+      </c>
+      <c r="AN5" s="3" t="n">
+        <v>0.00066473</v>
+      </c>
+      <c r="AO5" s="4" t="n">
+        <f aca="false">AN5/AM5</f>
+        <v>1.89020957147326</v>
+      </c>
+      <c r="AQ5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR5" s="6" t="n">
+        <v>42981</v>
+      </c>
+      <c r="AS5" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AT5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU5" s="3" t="n">
+        <v>0.00011663</v>
+      </c>
+      <c r="AV5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW5" s="0"/>
+      <c r="AX5" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="AY5" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="AZ5" s="1" t="n">
+        <v>61</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>9.74</v>
@@ -672,10 +1070,10 @@
         <v>8.34</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>50</v>
+        <v>83</v>
       </c>
       <c r="M6" s="3" t="n">
         <v>5.8032E-005</v>
@@ -684,10 +1082,10 @@
         <v>5.9841E-005</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="V6" s="1" t="n">
         <v>0.6268617</v>
@@ -705,19 +1103,87 @@
         <f aca="false">AVERAGE(V6:Y6)</f>
         <v>0.783025525</v>
       </c>
-      <c r="AC6" s="1" t="n">
+      <c r="AB6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK6" s="2" t="n">
         <v>40000</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="3" t="n">
+        <v>0.00032766</v>
+      </c>
+      <c r="AN6" s="3" t="n">
+        <v>0.00074182</v>
+      </c>
+      <c r="AO6" s="4" t="n">
+        <f aca="false">AN6/AM6</f>
+        <v>2.26399316364524</v>
+      </c>
+      <c r="AQ6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AR6" s="6" t="n">
+        <v>42981</v>
+      </c>
+      <c r="AS6" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="AT6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU6" s="3" t="n">
+        <v>8.6601E-005</v>
+      </c>
+      <c r="AV6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW6" s="0"/>
+      <c r="AX6" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY6" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="AZ6" s="1" t="n">
+        <v>68</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>15.88</v>
@@ -739,10 +1205,10 @@
         <v>15.488</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>56</v>
+        <v>89</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="M7" s="3" t="n">
         <v>0.00011773</v>
@@ -751,30 +1217,70 @@
         <v>0.00012194</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC7" s="1" t="n">
-        <v>70000</v>
+        <v>91</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK7" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM7" s="3" t="n">
+        <v>0.000257</v>
+      </c>
+      <c r="AN7" s="3" t="n">
+        <v>0.00064</v>
+      </c>
+      <c r="AO7" s="4" t="n">
+        <f aca="false">AN7/AM7</f>
+        <v>2.49027237354086</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>64</v>
+        <v>97</v>
       </c>
       <c r="M8" s="3" t="n">
         <v>3.1948E-007</v>
@@ -797,6 +1303,1413 @@
       <c r="S8" s="1" t="n">
         <f aca="false">AVERAGE(O8:R8)</f>
         <v>0.6540372</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK8" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL8" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM8" s="3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="AN8" s="3" t="n">
+        <v>0.0016</v>
+      </c>
+      <c r="AO8" s="4" t="n">
+        <f aca="false">AN8/AM8</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK9" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM9" s="3" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="AN9" s="3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="AO9" s="4" t="n">
+        <f aca="false">AN9/AM9</f>
+        <v>0.909090909090909</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK10" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL10" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM10" s="3" t="n">
+        <v>0.0011</v>
+      </c>
+      <c r="AN10" s="3" t="n">
+        <v>0.0014</v>
+      </c>
+      <c r="AO10" s="4" t="n">
+        <f aca="false">AN10/AM10</f>
+        <v>1.27272727272727</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK11" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL11" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM11" s="3" t="n">
+        <v>0.00096</v>
+      </c>
+      <c r="AN11" s="3" t="n">
+        <v>0.0009565</v>
+      </c>
+      <c r="AO11" s="4" t="n">
+        <f aca="false">AN11/AM11</f>
+        <v>0.996354166666667</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK12" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM12" s="3" t="n">
+        <v>0.00095194</v>
+      </c>
+      <c r="AN12" s="3" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="AO12" s="4" t="n">
+        <f aca="false">AN12/AM12</f>
+        <v>1.05048637519171</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK13" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL13" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM13" s="3" t="n">
+        <v>0.00053373</v>
+      </c>
+      <c r="AN13" s="3" t="n">
+        <v>0.00070903</v>
+      </c>
+      <c r="AO13" s="4" t="n">
+        <f aca="false">AN13/AM13</f>
+        <v>1.32844322035486</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AC14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK14" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM14" s="3" t="n">
+        <v>0.00035654</v>
+      </c>
+      <c r="AN14" s="3" t="n">
+        <v>0.00051859</v>
+      </c>
+      <c r="AO14" s="4" t="n">
+        <f aca="false">AN14/AM14</f>
+        <v>1.45450720816739</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK15" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM15" s="3" t="n">
+        <v>0.00051584</v>
+      </c>
+      <c r="AN15" s="3" t="n">
+        <v>0.0005805</v>
+      </c>
+      <c r="AO15" s="4" t="n">
+        <f aca="false">AN15/AM15</f>
+        <v>1.12534894540943</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI16" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK16" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL16" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM16" s="3" t="n">
+        <v>0.00059604</v>
+      </c>
+      <c r="AN16" s="3" t="n">
+        <v>0.00073992</v>
+      </c>
+      <c r="AO16" s="4" t="n">
+        <f aca="false">AN16/AM16</f>
+        <v>1.24139319508758</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK17" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL17" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM17" s="3" t="n">
+        <v>0.00031962</v>
+      </c>
+      <c r="AN17" s="3" t="n">
+        <v>0.00058485</v>
+      </c>
+      <c r="AO17" s="4" t="n">
+        <f aca="false">AN17/AM17</f>
+        <v>1.82982917214192</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK18" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM18" s="3" t="n">
+        <v>0.00040305</v>
+      </c>
+      <c r="AN18" s="3" t="n">
+        <v>0.00046447</v>
+      </c>
+      <c r="AO18" s="4" t="n">
+        <f aca="false">AN18/AM18</f>
+        <v>1.15238804118596</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI19" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK19" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL19" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM19" s="3" t="n">
+        <v>0.00040988</v>
+      </c>
+      <c r="AN19" s="3" t="n">
+        <v>0.00040491</v>
+      </c>
+      <c r="AO19" s="4" t="n">
+        <f aca="false">AN19/AM19</f>
+        <v>0.987874499853616</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI20" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK20" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL20" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM20" s="3" t="n">
+        <v>0.00043469</v>
+      </c>
+      <c r="AN20" s="3" t="n">
+        <v>0.00046688</v>
+      </c>
+      <c r="AO20" s="4" t="n">
+        <f aca="false">AN20/AM20</f>
+        <v>1.0740527732407</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AJ21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK21" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM21" s="3" t="n">
+        <v>0.00043485</v>
+      </c>
+      <c r="AN21" s="3" t="n">
+        <v>0.00048646</v>
+      </c>
+      <c r="AO21" s="4" t="n">
+        <f aca="false">AN21/AM21</f>
+        <v>1.1186846038864</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI22" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="AJ22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK22" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL22" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM22" s="3" t="n">
+        <v>0.00049598</v>
+      </c>
+      <c r="AN22" s="3" t="n">
+        <v>0.00051548</v>
+      </c>
+      <c r="AO22" s="4" t="n">
+        <f aca="false">AN22/AM22</f>
+        <v>1.0393161014557</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC24" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH25" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK25" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL25" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM25" s="3" t="n">
+        <v>0.00034529</v>
+      </c>
+      <c r="AN25" s="3" t="n">
+        <v>0.00044411</v>
+      </c>
+      <c r="AO25" s="4" t="n">
+        <f aca="false">AN25/AM25</f>
+        <v>1.28619421355962</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD26" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH26" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI26" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK26" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL26" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM26" s="3" t="n">
+        <v>0.00038322</v>
+      </c>
+      <c r="AN26" s="3" t="n">
+        <v>0.00041623</v>
+      </c>
+      <c r="AO26" s="4" t="n">
+        <f aca="false">AN26/AM26</f>
+        <v>1.08613851051615</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC27" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG27" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH27" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK27" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL27" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM27" s="3" t="n">
+        <v>0.00051188</v>
+      </c>
+      <c r="AN27" s="3" t="n">
+        <v>0.00067746</v>
+      </c>
+      <c r="AO27" s="4" t="n">
+        <f aca="false">AN27/AM27</f>
+        <v>1.32347425177776</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD28" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH28" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI28" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK28" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL28" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM28" s="3" t="n">
+        <v>0.00056771</v>
+      </c>
+      <c r="AN28" s="3" t="n">
+        <v>0.00056901</v>
+      </c>
+      <c r="AO28" s="4" t="n">
+        <f aca="false">AN28/AM28</f>
+        <v>1.00228990153423</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH29" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI29" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK29" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL29" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM29" s="3" t="n">
+        <v>0.00055576</v>
+      </c>
+      <c r="AN29" s="3" t="n">
+        <v>0.00071184</v>
+      </c>
+      <c r="AO29" s="4" t="n">
+        <f aca="false">AN29/AM29</f>
+        <v>1.28084065064056</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AO30" s="4"/>
+    </row>
+    <row r="31" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AO31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI32" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK32" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL32" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM32" s="3" t="n">
+        <v>0.00038915</v>
+      </c>
+      <c r="AN32" s="3" t="n">
+        <v>0.00050402</v>
+      </c>
+      <c r="AO32" s="4" t="n">
+        <f aca="false">AN32/AM32</f>
+        <v>1.29518180650135</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC33" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF33" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH33" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI33" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK33" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="AL33" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM33" s="3" t="n">
+        <v>0.00023753</v>
+      </c>
+      <c r="AN33" s="3" t="n">
+        <v>0.00037165</v>
+      </c>
+      <c r="AO33" s="4" t="n">
+        <f aca="false">AN33/AM33</f>
+        <v>1.56464446596219</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI34" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK34" s="2" t="n">
+        <v>40000</v>
+      </c>
+      <c r="AL34" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM34" s="3" t="n">
+        <v>0.00033731</v>
+      </c>
+      <c r="AN34" s="3" t="n">
+        <v>0.00040233</v>
+      </c>
+      <c r="AO34" s="4" t="n">
+        <f aca="false">AN34/AM34</f>
+        <v>1.19276036880021</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI35" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK35" s="2" t="n">
+        <v>40000</v>
+      </c>
+      <c r="AL35" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM35" s="3" t="n">
+        <v>0.00019563</v>
+      </c>
+      <c r="AN35" s="3" t="n">
+        <v>0.00032243</v>
+      </c>
+      <c r="AO35" s="4" t="n">
+        <f aca="false">AN35/AM35</f>
+        <v>1.64816234728825</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI36" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK36" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL36" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM36" s="3" t="n">
+        <v>0.00024444</v>
+      </c>
+      <c r="AN36" s="3" t="n">
+        <v>0.0002905</v>
+      </c>
+      <c r="AO36" s="4" t="n">
+        <f aca="false">AN36/AM36</f>
+        <v>1.18843069873998</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI37" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ37" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK37" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL37" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM37" s="3" t="n">
+        <v>0.00012216</v>
+      </c>
+      <c r="AN37" s="3" t="n">
+        <v>0.00019744</v>
+      </c>
+      <c r="AO37" s="4" t="n">
+        <f aca="false">AN37/AM37</f>
+        <v>1.61624099541585</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC39" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI40" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ40" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK40" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL40" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM40" s="3" t="n">
+        <v>0.00013272</v>
+      </c>
+      <c r="AN40" s="3" t="n">
+        <v>0.00020774</v>
+      </c>
+      <c r="AO40" s="4" t="n">
+        <f aca="false">AN40/AM40</f>
+        <v>1.56525015069319</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC41" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH41" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI41" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ41" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK41" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL41" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM41" s="3" t="n">
+        <v>3.1931E-005</v>
+      </c>
+      <c r="AN41" s="3" t="n">
+        <v>0.00013674</v>
+      </c>
+      <c r="AO41" s="4" t="n">
+        <f aca="false">AN41/AM41</f>
+        <v>4.28235883624064</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF42" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG42" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH42" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI42" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ42" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK42" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL42" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM42" s="3" t="n">
+        <v>0.00016925</v>
+      </c>
+      <c r="AN42" s="3" t="n">
+        <v>0.00019271</v>
+      </c>
+      <c r="AO42" s="4" t="n">
+        <f aca="false">AN42/AM42</f>
+        <v>1.13861152141802</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC43" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ43" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK43" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL43" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM43" s="3" t="n">
+        <v>6.041E-005</v>
+      </c>
+      <c r="AN43" s="3" t="n">
+        <v>0.0001029</v>
+      </c>
+      <c r="AO43" s="4" t="n">
+        <f aca="false">AN43/AM43</f>
+        <v>1.70336037079954</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC44" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI44" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK44" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL44" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="AM44" s="3" t="n">
+        <v>2.5002E-005</v>
+      </c>
+      <c r="AN44" s="3" t="n">
+        <v>7.6678E-005</v>
+      </c>
+      <c r="AO44" s="4" t="n">
+        <f aca="false">AN44/AM44</f>
+        <v>3.066874650028</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC45" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG45" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AH45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI45" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ45" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AK45" s="2" t="n">
+        <v>70008</v>
+      </c>
+      <c r="AL45" s="2" t="n">
+        <v>150</v>
+      </c>
+      <c r="AM45" s="3" t="n">
+        <v>1.5688E-005</v>
+      </c>
+      <c r="AN45" s="3" t="n">
+        <v>6.9595E-005</v>
+      </c>
+      <c r="AO45" s="4" t="n">
+        <f aca="false">AN45/AM45</f>
+        <v>4.43619326874044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>